<commit_message>
update chronology of datasheet
</commit_message>
<xml_diff>
--- a/analysis/data/Supplementary_Information/KWL_layer_assign_details.xlsx
+++ b/analysis/data/Supplementary_Information/KWL_layer_assign_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/Supplementary_Information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAC19A9-7E35-AE42-8CCB-B3CF28EE3C27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82C1B0A-97CD-1E45-9C77-1AF4988E8798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="1240" windowWidth="28300" windowHeight="16540" xr2:uid="{8078604F-F89D-654A-983C-649D14E5F3E8}"/>
+    <workbookView xWindow="500" yWindow="480" windowWidth="28300" windowHeight="16540" xr2:uid="{8078604F-F89D-654A-983C-649D14E5F3E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="207">
   <si>
     <t>L1</t>
   </si>
@@ -83,33 +83,21 @@
     <t>P041</t>
   </si>
   <si>
-    <t>jar pieces in L7&lt; 10g</t>
-  </si>
-  <si>
     <t>P042</t>
   </si>
   <si>
     <t>more potsherds in L1, L2</t>
   </si>
   <si>
-    <t>big pieces of jar in L2, L3, disturbed to 0 cm, contradicts the strategraphy</t>
-  </si>
-  <si>
     <t>P051</t>
   </si>
   <si>
     <t>P052</t>
   </si>
   <si>
-    <t>burial date contradicts other resutls, small piece of jar in L8 &lt;15g, and could be alluvial layer</t>
-  </si>
-  <si>
     <t>P053</t>
   </si>
   <si>
-    <t>pieces in L9-L12 could come from middens</t>
-  </si>
-  <si>
     <t>P054</t>
   </si>
   <si>
@@ -413,12 +401,6 @@
     <t>the earliest layer with diagnostic items</t>
   </si>
   <si>
-    <t>more artifacts and charcols in L10</t>
-  </si>
-  <si>
-    <t>sw: black color in L7, more pots</t>
-  </si>
-  <si>
     <t>more charcoals and local potsherds in L6 and L7</t>
   </si>
   <si>
@@ -464,9 +446,6 @@
     <t>more potsherds and charcols in L5 and L6</t>
   </si>
   <si>
-    <t>disturbed, C14 dating seems not reliable. Small pieces in L12</t>
-  </si>
-  <si>
     <t>big pieces of jar in L5 that contradicts the strategraphical data</t>
   </si>
   <si>
@@ -566,12 +545,6 @@
     <t>The start of Chinese phase (19th)</t>
   </si>
   <si>
-    <t>L14</t>
-  </si>
-  <si>
-    <t>Increasing charcoals and potsherds in L6</t>
-  </si>
-  <si>
     <t>assigning chronology</t>
   </si>
   <si>
@@ -582,6 +555,105 @@
   </si>
   <si>
     <t>European phase indicated by Anping jar in L7 accompied with more potsherds</t>
+  </si>
+  <si>
+    <t>L5, L6</t>
+  </si>
+  <si>
+    <t>L6, L7</t>
+  </si>
+  <si>
+    <t>L7, L8</t>
+  </si>
+  <si>
+    <t>L8, L9</t>
+  </si>
+  <si>
+    <t>L6, L7, L8, L9</t>
+  </si>
+  <si>
+    <t>L7, L8, L9</t>
+  </si>
+  <si>
+    <t>L3, L4</t>
+  </si>
+  <si>
+    <t>L9, L10</t>
+  </si>
+  <si>
+    <t>L6, L7, L8</t>
+  </si>
+  <si>
+    <t>L6,L7</t>
+  </si>
+  <si>
+    <t>L4, L5</t>
+  </si>
+  <si>
+    <t>L5, L6, L7</t>
+  </si>
+  <si>
+    <t>previous studies indicating 17th layer</t>
+  </si>
+  <si>
+    <t>L2, L3</t>
+  </si>
+  <si>
+    <t>L2, L3, L4</t>
+  </si>
+  <si>
+    <t>L4, L5, L6</t>
+  </si>
+  <si>
+    <t>L3, L4, L5, L6</t>
+  </si>
+  <si>
+    <t>L1, L2</t>
+  </si>
+  <si>
+    <t>L1, L2, L3</t>
+  </si>
+  <si>
+    <t>previous studies indicating 19th layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">small jar pieces in L7&lt; 10g, likely postdepositional disturbance </t>
+  </si>
+  <si>
+    <t>big pieces of jar in L2, L3, disturbed to 0 cm</t>
+  </si>
+  <si>
+    <t>European phase indicated by more pieces of Anping jars in L5 with the references of more potsherds and radiocarbon date</t>
+  </si>
+  <si>
+    <t>European phase indicated by more pieces of Anping jars and pipe in L1 with the references of connection with P041</t>
+  </si>
+  <si>
+    <t>more artifacts and charcols in L10-L11</t>
+  </si>
+  <si>
+    <t>European phase indicated by more pieces of Anping jars and pipe in L11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C14 dates seem not very reasonable indicating distrubance or camtamination of samples. Small pieces of jar in L12, , likely postdepositional disturbance </t>
+  </si>
+  <si>
+    <t>burial date contradicts other rediocarbon dates, possibly old wood effect or a alluvial layer</t>
+  </si>
+  <si>
+    <t>increasing charcoals and potsherds beginning from L6, color changes to darker in L8</t>
+  </si>
+  <si>
+    <t>color changes in L8 with a wide vaireity of artifacts</t>
+  </si>
+  <si>
+    <t>jar pieces in L9-L12 likely from middens</t>
+  </si>
+  <si>
+    <t>European phase indicated by Anping jars and colar change in L8 with the referrence of radiocarbon date of L7</t>
+  </si>
+  <si>
+    <t>European phase indicated by Anping jars and colar change in L8</t>
   </si>
 </sst>
 </file>
@@ -623,7 +695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -636,6 +708,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -950,28 +1023,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B88541E-9DAB-0E45-BDCD-701CF40445C7}">
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="I6" zoomScale="125" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.1640625" style="1" customWidth="1"/>
-    <col min="2" max="14" width="10.83203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="14.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="1" customWidth="1"/>
+    <col min="3" max="14" width="10.83203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5" style="1" customWidth="1"/>
     <col min="16" max="16" width="24" style="2" customWidth="1"/>
     <col min="17" max="17" width="29" style="2" customWidth="1"/>
-    <col min="18" max="19" width="30.1640625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="15.33203125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="10.6640625" style="2" customWidth="1"/>
-    <col min="22" max="16384" width="10.83203125" style="1"/>
+    <col min="18" max="18" width="28.1640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="10.83203125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="10.83203125" style="1"/>
+    <col min="21" max="21" width="35.5" style="1" customWidth="1"/>
+    <col min="22" max="22" width="11.83203125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="10.6640625" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="68" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1013,384 +1090,457 @@
         <v>12</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>162</v>
+        <v>193</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="T2" s="2">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="U2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="V2" s="2">
+        <v>1</v>
+      </c>
+      <c r="W2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+      <c r="X2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="R3" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="V3" s="2">
+        <v>1</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2">
-        <v>1</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="B4" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="V4" s="4">
+        <v>3</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="T4" s="4">
-        <v>3</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="J5" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="T5" s="2">
-        <v>1</v>
+        <v>198</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="V5" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="V5" s="2">
+        <v>1</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="X5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2">
-        <v>1</v>
+        <v>201</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="U6" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="V6" s="2">
+        <v>1</v>
+      </c>
+      <c r="W6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="X6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="M7" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>127</v>
+        <v>203</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T7" s="2">
-        <v>1</v>
+        <v>204</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="U7" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="V7" s="2">
+        <v>1</v>
+      </c>
+      <c r="W7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="T8" s="2">
+        <v>137</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V8" s="2">
         <v>2</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="W8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="X8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="T9" s="2">
-        <v>1</v>
-      </c>
-      <c r="U9" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V9" s="2">
+        <v>1</v>
+      </c>
+      <c r="W9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="V9" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="X9" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="T10" s="2">
-        <v>1</v>
-      </c>
-      <c r="U10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="V10" s="2">
+        <v>1</v>
+      </c>
+      <c r="W10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="I11" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="N11" s="1">
         <v>1</v>
@@ -1399,172 +1549,196 @@
         <v>12</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2">
-        <v>1</v>
-      </c>
-      <c r="U11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2">
+        <v>1</v>
+      </c>
+      <c r="W11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="X11" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T12" s="2">
-        <v>1</v>
-      </c>
-      <c r="U12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="V12" s="2">
+        <v>1</v>
+      </c>
+      <c r="W12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="X12" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T13" s="2">
-        <v>1</v>
-      </c>
-      <c r="U13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="V13" s="2">
+        <v>1</v>
+      </c>
+      <c r="W13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="V13" s="1" t="s">
+      <c r="X13" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="T14" s="2">
-        <v>1</v>
-      </c>
-      <c r="U14" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="V14" s="2">
+        <v>1</v>
+      </c>
+      <c r="W14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="V14" s="1" t="s">
+      <c r="X14" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="N15" s="1">
         <v>1</v>
@@ -1573,1001 +1747,1169 @@
         <v>12</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2">
-        <v>1</v>
-      </c>
-      <c r="U15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2">
+        <v>1</v>
+      </c>
+      <c r="W15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="V15" s="1" t="s">
+      <c r="X15" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2">
-        <v>1</v>
-      </c>
-      <c r="U16" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="S16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V16" s="1" t="s">
+      <c r="T16" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="U16" s="2"/>
+      <c r="V16" s="2">
+        <v>1</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2">
-        <v>1</v>
-      </c>
-      <c r="U17" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2">
+        <v>1</v>
+      </c>
+      <c r="W17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="V17" s="1" t="s">
+      <c r="X17" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>4</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T18" s="2">
-        <v>1</v>
-      </c>
-      <c r="U18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V18" s="2">
+        <v>1</v>
+      </c>
+      <c r="W18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="V18" s="1" t="s">
+      <c r="X18" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="T19" s="2">
-        <v>1</v>
-      </c>
-      <c r="U19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="V19" s="1" t="s">
+      <c r="T19" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="V19" s="2">
+        <v>1</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2">
-        <v>1</v>
-      </c>
-      <c r="U20" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2">
+        <v>1</v>
+      </c>
+      <c r="W20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="V20" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="X20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>9</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="T21" s="2">
-        <v>1</v>
-      </c>
-      <c r="U21" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="V21" s="2">
+        <v>1</v>
+      </c>
+      <c r="W21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="V21" s="1" t="s">
+      <c r="X21" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="T22" s="2">
-        <v>1</v>
-      </c>
-      <c r="U22" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="V22" s="2">
+        <v>1</v>
+      </c>
+      <c r="W22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="V22" s="1" t="s">
+      <c r="X22" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="T23" s="2">
-        <v>1</v>
-      </c>
-      <c r="U23" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="V23" s="2">
+        <v>1</v>
+      </c>
+      <c r="W23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="V23" s="1" t="s">
+      <c r="X23" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="T24" s="2">
-        <v>1</v>
-      </c>
-      <c r="U24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="V24" s="2">
+        <v>1</v>
+      </c>
+      <c r="W24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="V24" s="1" t="s">
+      <c r="X24" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>10</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="T25" s="2">
-        <v>1</v>
-      </c>
-      <c r="U25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="V25" s="2">
+        <v>1</v>
+      </c>
+      <c r="W25" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="V25" s="1" t="s">
+      <c r="X25" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2">
-        <v>1</v>
-      </c>
-      <c r="U26" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="S26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V26" s="1" t="s">
+      <c r="T26" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2">
+        <v>1</v>
+      </c>
+      <c r="W26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X26" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="T27" s="2">
-        <v>1</v>
-      </c>
-      <c r="U27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="V27" s="1" t="s">
+      <c r="T27" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="V27" s="2">
+        <v>1</v>
+      </c>
+      <c r="W27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="X27" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="T28" s="2">
-        <v>1</v>
-      </c>
-      <c r="U28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="V28" s="2">
+        <v>1</v>
+      </c>
+      <c r="W28" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="V28" s="1" t="s">
+      <c r="X28" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>4</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="T29" s="2">
-        <v>1</v>
-      </c>
-      <c r="U29" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V29" s="2">
+        <v>1</v>
+      </c>
+      <c r="W29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V29" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="X29" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="O30" s="3" t="s">
         <v>1</v>
       </c>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="R30" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="S30" s="4"/>
-      <c r="T30" s="4">
+        <v>153</v>
+      </c>
+      <c r="S30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="T30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4">
         <v>3</v>
       </c>
-      <c r="U30" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="V30" s="3" t="s">
+      <c r="W30" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X30" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="O31" s="1" t="s">
         <v>4</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="T31" s="2">
-        <v>1</v>
-      </c>
-      <c r="U31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="S31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V31" s="2">
+        <v>1</v>
+      </c>
+      <c r="W31" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="V31" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="X31" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="O32" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Q32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="S32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V32" s="2">
+        <v>1</v>
+      </c>
+      <c r="W32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X32" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R33" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="R32" s="1" t="s">
+      <c r="S33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V33" s="2">
+        <v>2</v>
+      </c>
+      <c r="W33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="X33" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="T32" s="2">
-        <v>1</v>
-      </c>
-      <c r="U32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="V32" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q33" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="T33" s="2">
-        <v>2</v>
-      </c>
-      <c r="U33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="V33" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="O34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="T34" s="2">
+        <v>75</v>
+      </c>
+      <c r="S34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="U34" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="V34" s="1" t="s">
+      <c r="T34" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="V34" s="2">
+        <v>2</v>
+      </c>
+      <c r="W34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="X34" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="T35" s="2">
-        <v>1</v>
-      </c>
-      <c r="U35" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="S35" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="V35" s="2">
+        <v>1</v>
+      </c>
+      <c r="W35" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V35" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="X35" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O36" s="1" t="s">
         <v>6</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2">
-        <v>1</v>
-      </c>
-      <c r="U36" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="S36" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="V36" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="T36" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2">
+        <v>1</v>
+      </c>
+      <c r="W36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="X36" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="O37" s="1" t="s">
         <v>9</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="T37" s="2">
-        <v>1</v>
-      </c>
-      <c r="U37" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="S37" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="V37" s="2">
+        <v>1</v>
+      </c>
+      <c r="W37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="V37" s="1" t="s">
+      <c r="X37" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:24" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="S38" s="2"/>
-      <c r="T38" s="2">
-        <v>1</v>
-      </c>
-      <c r="U38" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="S38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T38" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2">
+        <v>1</v>
+      </c>
+      <c r="W38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="V38" s="1" t="s">
+      <c r="X38" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="O39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="T39" s="2">
-        <v>1</v>
-      </c>
-      <c r="U39" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="S39" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="T39" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="V39" s="2">
+        <v>1</v>
+      </c>
+      <c r="W39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="V39" s="1" t="s">
+      <c r="X39" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="O40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="S40" s="2"/>
-      <c r="T40" s="2">
-        <v>1</v>
-      </c>
-      <c r="U40" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="S40" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="T40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2">
+        <v>1</v>
+      </c>
+      <c r="W40" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="V40" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="X40" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="O41" s="1" t="s">
         <v>9</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="S41" s="2"/>
-      <c r="T41" s="2">
-        <v>1</v>
-      </c>
-      <c r="U41" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="S41" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="T41" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="U41" s="2"/>
+      <c r="V41" s="2">
+        <v>1</v>
+      </c>
+      <c r="W41" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="V41" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+      <c r="X41" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="O42" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="T42" s="2">
+        <v>146</v>
+      </c>
+      <c r="S42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V42" s="2">
         <v>2</v>
       </c>
-      <c r="U42" s="2" t="s">
+      <c r="W42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V42" s="1" t="s">
+      <c r="X42" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add tiles and bricks data to datasheet file
</commit_message>
<xml_diff>
--- a/analysis/data/Supplementary_Information/KWL_layer_assign_details.xlsx
+++ b/analysis/data/Supplementary_Information/KWL_layer_assign_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/Supplementary_Information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F649BFCB-6D01-224D-A96B-F9BC2B43C2F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E9C9F0-29D2-3143-8384-9C667610CA5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="480" windowWidth="28300" windowHeight="16540" xr2:uid="{8078604F-F89D-654A-983C-649D14E5F3E8}"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="28300" windowHeight="16540" xr2:uid="{8078604F-F89D-654A-983C-649D14E5F3E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="255">
   <si>
     <t>L1</t>
   </si>
@@ -302,12 +302,6 @@
     <t>pipe*1, jar*4, stoneware*1</t>
   </si>
   <si>
-    <t>jar*1, stoneware*2</t>
-  </si>
-  <si>
-    <t>jar*1, stoneware*1</t>
-  </si>
-  <si>
     <t>pipe*2, jar*7</t>
   </si>
   <si>
@@ -756,13 +750,61 @@
   </si>
   <si>
     <t>assigning the layer indicating the start of European phase</t>
+  </si>
+  <si>
+    <t>assigning the layer indicating the start of Chinese phase</t>
+  </si>
+  <si>
+    <t>tile</t>
+  </si>
+  <si>
+    <t>tile, jar*2</t>
+  </si>
+  <si>
+    <t>bricks</t>
+  </si>
+  <si>
+    <t>tiles</t>
+  </si>
+  <si>
+    <t>bricks, jar*1, stoneware*2</t>
+  </si>
+  <si>
+    <t>tiles, jar*1</t>
+  </si>
+  <si>
+    <t>tiles, jar*1, stoneware*1</t>
+  </si>
+  <si>
+    <t>tiles, pipe*1</t>
+  </si>
+  <si>
+    <t>tiles, jar*2</t>
+  </si>
+  <si>
+    <t>tiles, bricks</t>
+  </si>
+  <si>
+    <t>bricks, jar*1</t>
+  </si>
+  <si>
+    <t>tiles, brciks, jar*2</t>
+  </si>
+  <si>
+    <t>tiles, bricks, jar*1, stoneware*1</t>
+  </si>
+  <si>
+    <t>tiles, pipe*1, jar*1</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L1 that continue to L2 according to soil color</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -773,6 +815,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -797,7 +845,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -811,6 +859,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1125,10 +1174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B88541E-9DAB-0E45-BDCD-701CF40445C7}">
-  <dimension ref="A1:X42"/>
+  <dimension ref="A1:Y42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1143,12 +1192,12 @@
     <col min="19" max="19" width="11.83203125" style="2" customWidth="1"/>
     <col min="20" max="20" width="10.83203125" style="2" customWidth="1"/>
     <col min="21" max="21" width="10.83203125" style="1"/>
-    <col min="22" max="22" width="35.5" style="1" customWidth="1"/>
-    <col min="23" max="23" width="10.6640625" style="2" customWidth="1"/>
-    <col min="24" max="16384" width="10.83203125" style="1"/>
+    <col min="22" max="23" width="35.5" style="1" customWidth="1"/>
+    <col min="24" max="24" width="10.6640625" style="2" customWidth="1"/>
+    <col min="25" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
@@ -1192,40 +1241,46 @@
         <v>12</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="R1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+      <c r="Y1" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="F2" s="1" t="s">
         <v>65</v>
       </c>
@@ -1242,10 +1297,10 @@
         <v>8</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="S2" s="2">
         <v>1</v>
@@ -1257,16 +1312,19 @@
         <v>14</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="W2" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="X2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+      <c r="Y2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1289,13 +1347,13 @@
         <v>7</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="S3" s="2">
         <v>1</v>
@@ -1307,16 +1365,17 @@
         <v>14</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="W3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -1337,7 +1396,7 @@
         <v>49</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="S4" s="4">
         <v>3</v>
@@ -1349,19 +1408,23 @@
         <v>14</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="W4" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="W4" s="2"/>
+      <c r="X4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="J5" s="1" t="s">
         <v>65</v>
       </c>
@@ -1375,13 +1438,13 @@
         <v>11</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q5" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="R5" s="6" t="s">
         <v>141</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>143</v>
       </c>
       <c r="S5" s="2">
         <v>1</v>
@@ -1393,19 +1456,26 @@
         <v>14</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="W5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="Y5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="F6" s="1" t="s">
         <v>80</v>
       </c>
@@ -1419,13 +1489,13 @@
         <v>7</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="S6" s="2">
         <v>1</v>
@@ -1437,16 +1507,17 @@
         <v>14</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="W6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="Y6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -1478,10 +1549,10 @@
         <v>11</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="S7" s="2">
         <v>1</v>
@@ -1493,16 +1564,17 @@
         <v>14</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="W7" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="Y7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1525,10 +1597,10 @@
         <v>5</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="S8" s="2">
         <v>2</v>
@@ -1540,16 +1612,17 @@
         <v>14</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="W8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="Y8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1566,31 +1639,32 @@
         <v>5</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="S9" s="2">
         <v>1</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="W9" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X9" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y9" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1601,7 +1675,7 @@
         <v>65</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>73</v>
@@ -1610,7 +1684,7 @@
         <v>6</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>23</v>
@@ -1619,22 +1693,23 @@
         <v>1</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="W10" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="X10" s="1" t="s">
+      <c r="Y10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -1663,31 +1738,41 @@
         <v>25</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="S11" s="2">
         <v>1</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="W11" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="X11" s="1" t="s">
+      <c r="Y11" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="F12" s="1" t="s">
         <v>66</v>
       </c>
@@ -1710,36 +1795,46 @@
         <v>9</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="S12" s="2">
         <v>1</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="W12" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="X12" s="1" t="s">
+      <c r="Y12" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="E13" s="1" t="s">
-        <v>70</v>
+        <v>241</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>73</v>
@@ -1760,37 +1855,41 @@
         <v>9</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="S13" s="2">
         <v>1</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="W13" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="X13" s="1" t="s">
+      <c r="Y13" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="D14" s="1" t="s">
+        <v>240</v>
+      </c>
       <c r="H14" s="1" t="s">
         <v>70</v>
       </c>
@@ -1813,37 +1912,41 @@
         <v>11</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>29</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="S14" s="2">
         <v>1</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="W14" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="X14" s="1" t="s">
+      <c r="Y14" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="G15" s="1" t="s">
         <v>70</v>
       </c>
@@ -1869,36 +1972,46 @@
         <v>12</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="S15" s="2">
         <v>1</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="W15" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="X15" s="1" t="s">
+      <c r="Y15" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>242</v>
+      </c>
       <c r="F16" s="1" t="s">
-        <v>89</v>
+        <v>244</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>66</v>
@@ -1910,7 +2023,7 @@
         <v>43</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="S16" s="2">
         <v>1</v>
@@ -1922,24 +2035,31 @@
         <v>2</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="W16" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="X16" s="1" t="s">
+      <c r="Y16" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="B17" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="D17" s="1" t="s">
-        <v>66</v>
+        <v>245</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>90</v>
+        <v>246</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>66</v>
@@ -1960,37 +2080,41 @@
         <v>11</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="S17" s="2">
         <v>1</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="U17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="W17" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="X17" s="1" t="s">
+      <c r="Y17" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="B18" s="7" t="s">
+        <v>243</v>
+      </c>
       <c r="C18" s="1" t="s">
         <v>66</v>
       </c>
@@ -2001,7 +2125,7 @@
         <v>4</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="R18" s="1" t="s">
         <v>34</v>
@@ -2010,25 +2134,29 @@
         <v>1</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="W18" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="X18" s="1" t="s">
+      <c r="Y18" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="B19" s="7" t="s">
+        <v>243</v>
+      </c>
       <c r="D19" s="1" t="s">
         <v>66</v>
       </c>
@@ -2036,13 +2164,13 @@
         <v>2</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="Q19" s="2" t="s">
         <v>36</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="S19" s="2">
         <v>1</v>
@@ -2054,16 +2182,17 @@
         <v>0</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="W19" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="X19" s="1" t="s">
+      <c r="Y19" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
@@ -2089,42 +2218,46 @@
         <v>9</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="S20" s="2">
         <v>1</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="U20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="W20" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X20" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="B21" s="7" t="s">
+        <v>243</v>
+      </c>
       <c r="D21" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>67</v>
@@ -2142,39 +2275,49 @@
         <v>9</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="S21" s="2">
         <v>1</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="W21" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="X21" s="1" t="s">
+      <c r="Y21" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="B22" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>243</v>
+      </c>
       <c r="E22" s="1" t="s">
-        <v>66</v>
+        <v>245</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>65</v>
+        <v>247</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>243</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>74</v>
@@ -2189,16 +2332,16 @@
         <v>71</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="S22" s="2">
         <v>1</v>
@@ -2207,24 +2350,37 @@
         <v>9</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="W22" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="X22" s="1" t="s">
+      <c r="Y22" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="B23" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>243</v>
+      </c>
       <c r="E23" s="1" t="s">
-        <v>66</v>
+        <v>245</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>243</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>65</v>
@@ -2251,34 +2407,44 @@
         <v>11</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="S23" s="2">
         <v>1</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="W23" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="X23" s="1" t="s">
+      <c r="Y23" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="B24" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>243</v>
+      </c>
       <c r="I24" s="1" t="s">
         <v>66</v>
       </c>
@@ -2286,42 +2452,49 @@
         <v>7</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="S24" s="2">
         <v>1</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="W24" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="X24" s="1" t="s">
+      <c r="Y24" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="B25" s="7" t="s">
+        <v>243</v>
+      </c>
       <c r="C25" s="1" t="s">
-        <v>66</v>
+        <v>245</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>66</v>
+        <v>245</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>66</v>
+        <v>245</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>243</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>66</v>
@@ -2336,34 +2509,47 @@
         <v>10</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="S25" s="2">
         <v>1</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="W25" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X25" s="1" t="s">
+      <c r="Y25" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="B26" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>243</v>
+      </c>
       <c r="F26" s="1" t="s">
         <v>66</v>
       </c>
@@ -2374,10 +2560,10 @@
         <v>5</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="S26" s="2">
         <v>1</v>
@@ -2386,24 +2572,34 @@
         <v>4</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="V26" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="W26" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="X26" s="1" t="s">
+      <c r="Y26" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="B27" s="7" t="s">
+        <v>243</v>
+      </c>
       <c r="C27" s="1" t="s">
-        <v>65</v>
+        <v>247</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>243</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>66</v>
@@ -2412,7 +2608,7 @@
         <v>6</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R27" s="1" t="s">
         <v>23</v>
@@ -2424,19 +2620,20 @@
         <v>6</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="V27" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="W27" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="X27" s="1" t="s">
+      <c r="Y27" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
@@ -2453,7 +2650,7 @@
         <v>6</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="R28" s="1" t="s">
         <v>23</v>
@@ -2462,25 +2659,32 @@
         <v>1</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="V28" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="W28" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="X28" s="1" t="s">
+      <c r="Y28" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="B29" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>243</v>
+      </c>
       <c r="D29" s="1" t="s">
         <v>70</v>
       </c>
@@ -2494,46 +2698,50 @@
         <v>4</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="S29" s="2">
         <v>1</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="V29" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="W29" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="X29" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="Y29" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="B30" s="3" t="s">
+        <v>243</v>
+      </c>
       <c r="C30" s="3" t="s">
-        <v>70</v>
+        <v>248</v>
       </c>
       <c r="O30" s="3" t="s">
         <v>1</v>
       </c>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="R30" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="S30" s="4">
         <v>3</v>
@@ -2545,19 +2753,26 @@
         <v>14</v>
       </c>
       <c r="V30" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="W30" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="X30" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="W30" s="2"/>
+      <c r="X30" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y30" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="B31" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>243</v>
+      </c>
       <c r="D31" s="1" t="s">
         <v>65</v>
       </c>
@@ -2574,7 +2789,7 @@
         <v>51</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S31" s="2">
         <v>1</v>
@@ -2586,21 +2801,22 @@
         <v>14</v>
       </c>
       <c r="V31" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="W31" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="X31" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+      <c r="Y31" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>66</v>
@@ -2624,7 +2840,7 @@
         <v>53</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="S32" s="2">
         <v>1</v>
@@ -2636,16 +2852,17 @@
         <v>14</v>
       </c>
       <c r="V32" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="W32" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="X32" s="1" t="s">
+      <c r="Y32" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>54</v>
       </c>
@@ -2653,16 +2870,16 @@
         <v>66</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="S33" s="2">
         <v>2</v>
@@ -2674,19 +2891,23 @@
         <v>0</v>
       </c>
       <c r="V33" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="W33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="X33" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y33" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="B34" s="1" t="s">
+        <v>242</v>
+      </c>
       <c r="D34" s="1" t="s">
         <v>65</v>
       </c>
@@ -2697,10 +2918,10 @@
         <v>3</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="S34" s="2">
         <v>2</v>
@@ -2712,24 +2933,28 @@
         <v>0</v>
       </c>
       <c r="V34" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="W34" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="X34" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="B35" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="C35" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>85</v>
@@ -2744,31 +2969,32 @@
         <v>7</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="S35" s="2">
         <v>1</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U35" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="V35" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="W35" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="X35" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y35" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>57</v>
       </c>
@@ -2791,10 +3017,10 @@
         <v>6</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="S36" s="2">
         <v>1</v>
@@ -2803,24 +3029,25 @@
         <v>5</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="W36" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X36" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y36" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>90</v>
+        <v>246</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>66</v>
@@ -2841,34 +3068,38 @@
         <v>9</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="S37" s="2">
         <v>1</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="U37" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="V37" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="W37" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="X37" s="1" t="s">
+      <c r="Y37" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="85" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="B38" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="C38" s="1" t="s">
         <v>65</v>
       </c>
@@ -2897,13 +3128,13 @@
         <v>11</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S38" s="2">
         <v>1</v>
@@ -2912,24 +3143,28 @@
         <v>7</v>
       </c>
       <c r="U38" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="W38" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="X38" s="1" t="s">
+      <c r="Y38" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="B39" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="C39" s="1" t="s">
-        <v>66</v>
+        <v>250</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>70</v>
@@ -2953,39 +3188,46 @@
         <v>8</v>
       </c>
       <c r="Q39" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="R39" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="R39" s="1" t="s">
-        <v>214</v>
-      </c>
       <c r="S39" s="2">
         <v>1</v>
       </c>
       <c r="T39" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="U39" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="U39" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="V39" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="W39" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="X39" s="1" t="s">
+      <c r="Y39" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="B40" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="C40" s="1" t="s">
-        <v>70</v>
+        <v>251</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>90</v>
+        <v>252</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>66</v>
@@ -3000,34 +3242,38 @@
         <v>7</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="S40" s="2">
         <v>1</v>
       </c>
       <c r="T40" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="U40" s="1" t="s">
         <v>1</v>
       </c>
       <c r="V40" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="W40" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X40" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y40" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="B41" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="E41" s="1" t="s">
         <v>66</v>
       </c>
@@ -3044,39 +3290,40 @@
         <v>9</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="S41" s="2">
         <v>1</v>
       </c>
       <c r="T41" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="U41" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="V41" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="W41" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="W41" s="2"/>
+      <c r="X41" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="X41" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+      <c r="Y41" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>63</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>66</v>
+        <v>245</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>67</v>
+        <v>253</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>65</v>
@@ -3085,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="Q42" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="R42" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="R42" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="S42" s="2">
         <v>2</v>
@@ -3100,12 +3347,13 @@
         <v>14</v>
       </c>
       <c r="V42" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="W42" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="X42" s="1" t="s">
+      <c r="Y42" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edit the Chinese phase column
</commit_message>
<xml_diff>
--- a/analysis/data/Supplementary_Information/KWL_layer_assign_details.xlsx
+++ b/analysis/data/Supplementary_Information/KWL_layer_assign_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/Supplementary_Information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E9C9F0-29D2-3143-8384-9C667610CA5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A890A5-FDD6-204B-819B-3E5FE08B24D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="460" windowWidth="28300" windowHeight="16540" xr2:uid="{8078604F-F89D-654A-983C-649D14E5F3E8}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="256">
   <si>
     <t>L1</t>
   </si>
@@ -569,18 +569,9 @@
     <t>not many jars, river in the middle</t>
   </si>
   <si>
-    <t>European phase indicated by jar in L8 with the evidence of consistent color, context, and depth with adjecent units</t>
-  </si>
-  <si>
-    <t>European phase indicated by jar in L3 with the evidence of consistent color, context, and depth with adjecent units</t>
-  </si>
-  <si>
     <t>small piece of stoneware in L10, river in the middle</t>
   </si>
   <si>
-    <t>European phase indicated by jar in L6 with the evidence of consistent color, context, and depth with adjecent units</t>
-  </si>
-  <si>
     <t>more potsherds in L6-L8</t>
   </si>
   <si>
@@ -659,27 +650,15 @@
     <t>more potsherds and soil color turns black in L9</t>
   </si>
   <si>
-    <t>European phase indicated by pipe in L9 with the evidence of consistent color, and depth with adjecent units</t>
-  </si>
-  <si>
-    <t>European phase indicated by pipe in L5 with the evidence of consistent color, and depth with adjecent units</t>
-  </si>
-  <si>
     <t>more potsherds in L5-L7</t>
   </si>
   <si>
-    <t>European phase indicated by jar in L7 with the evidence of consistent color, artifacts, and depth with adjecent units</t>
-  </si>
-  <si>
     <t>pieces of jars in L8, liking coming from midden</t>
   </si>
   <si>
     <t>jar pieces in L8 &lt; 10g, likely postdepositional disturbance, and pieces in L7 might come from midden</t>
   </si>
   <si>
-    <t xml:space="preserve">European phase indicated by the consistent color, context, and depth of L6 with adjecent units, although no direct dignostic artifacts found </t>
-  </si>
-  <si>
     <t>more potsherds and charcols in L5-L6, darker soil color</t>
   </si>
   <si>
@@ -722,9 +701,6 @@
     <t>more local pots in L5</t>
   </si>
   <si>
-    <t>European phase indicated by jar in L5 with the evidence of consistent color, and depth with adjecent units</t>
-  </si>
-  <si>
     <t>one piece of jar in L6 &gt; 120g, likely postdepositional disturbance</t>
   </si>
   <si>
@@ -798,6 +774,33 @@
   </si>
   <si>
     <t>Chinese phase indicated by tiles in L1 that continue to L2 according to soil color</t>
+  </si>
+  <si>
+    <t>European phase indicated by jar in L3 with the evidence of consistent color, context, and depth with P071 and P085</t>
+  </si>
+  <si>
+    <t>European phase indicated by jar in L8 with the evidence of consistent color, context, and depth with P062</t>
+  </si>
+  <si>
+    <t>European phase indicated by pipe in L5 with the evidence of consistent color, and depth with P066 and P078</t>
+  </si>
+  <si>
+    <t>European phase indicated by pipe in L9 with the evidence of consistent color, and depth with P074, P088</t>
+  </si>
+  <si>
+    <t>European phase indicated by jar in L6 with the evidence of consistent color, context, and depth with P074 and P076</t>
+  </si>
+  <si>
+    <t>European phase indicated by jar in L7 with the evidence of consistent color, artifacts, and depth with P075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">European phase indicated by the consistent color, context, and depth of L6 with P092, although no direct dignostic artifacts found </t>
+  </si>
+  <si>
+    <t>European phase indicated by jar in L5 with the evidence of consistent color, and depth with P092 and P078</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by the consistent color, context, and depth of L1 with P040 and P042</t>
   </si>
 </sst>
 </file>
@@ -1176,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B88541E-9DAB-0E45-BDCD-701CF40445C7}">
   <dimension ref="A1:Y42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1262,10 +1265,10 @@
         <v>135</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>111</v>
@@ -1279,7 +1282,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>65</v>
@@ -1315,7 +1318,7 @@
         <v>115</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>6</v>
@@ -1353,7 +1356,7 @@
         <v>113</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="S3" s="2">
         <v>1</v>
@@ -1367,7 +1370,9 @@
       <c r="V3" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="W3" s="2"/>
+      <c r="W3" s="2" t="s">
+        <v>255</v>
+      </c>
       <c r="X3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1423,7 +1428,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>65</v>
@@ -1471,10 +1476,10 @@
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>80</v>
@@ -1597,7 +1602,7 @@
         <v>5</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>147</v>
@@ -1639,7 +1644,7 @@
         <v>5</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>150</v>
@@ -1684,7 +1689,7 @@
         <v>6</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>23</v>
@@ -1765,13 +1770,13 @@
         <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>66</v>
@@ -1795,7 +1800,7 @@
         <v>9</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>155</v>
@@ -1825,16 +1830,16 @@
         <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>73</v>
@@ -1855,7 +1860,7 @@
         <v>9</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>158</v>
@@ -1888,7 +1893,7 @@
         <v>66</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>70</v>
@@ -1918,7 +1923,7 @@
         <v>29</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="S14" s="2">
         <v>1</v>
@@ -1945,7 +1950,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>70</v>
@@ -1975,7 +1980,7 @@
         <v>161</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="S15" s="2">
         <v>1</v>
@@ -2002,16 +2007,16 @@
         <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>66</v>
@@ -2050,16 +2055,16 @@
         <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>66</v>
@@ -2086,7 +2091,7 @@
         <v>164</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="S17" s="2">
         <v>1</v>
@@ -2113,7 +2118,7 @@
         <v>33</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>66</v>
@@ -2125,7 +2130,7 @@
         <v>4</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="R18" s="1" t="s">
         <v>34</v>
@@ -2155,7 +2160,7 @@
         <v>35</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>66</v>
@@ -2182,7 +2187,7 @@
         <v>0</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>179</v>
+        <v>247</v>
       </c>
       <c r="W19" s="2"/>
       <c r="X19" s="2" t="s">
@@ -2218,7 +2223,7 @@
         <v>9</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="R20" s="2" t="s">
         <v>168</v>
@@ -2248,7 +2253,7 @@
         <v>38</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>65</v>
@@ -2305,19 +2310,19 @@
         <v>39</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>74</v>
@@ -2338,7 +2343,7 @@
         <v>12</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="R22" s="1" t="s">
         <v>174</v>
@@ -2368,19 +2373,19 @@
         <v>40</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>65</v>
@@ -2437,13 +2442,13 @@
         <v>41</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>66</v>
@@ -2452,7 +2457,7 @@
         <v>7</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="R24" s="1" t="s">
         <v>177</v>
@@ -2467,7 +2472,7 @@
         <v>129</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>178</v>
+        <v>248</v>
       </c>
       <c r="W24" s="2"/>
       <c r="X24" s="2" t="s">
@@ -2482,19 +2487,19 @@
         <v>42</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>66</v>
@@ -2509,10 +2514,10 @@
         <v>10</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="S25" s="2">
         <v>1</v>
@@ -2524,7 +2529,7 @@
         <v>129</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>181</v>
+        <v>251</v>
       </c>
       <c r="W25" s="2"/>
       <c r="X25" s="2" t="s">
@@ -2539,16 +2544,16 @@
         <v>44</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>66</v>
@@ -2560,10 +2565,10 @@
         <v>5</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="S26" s="2">
         <v>1</v>
@@ -2575,7 +2580,7 @@
         <v>129</v>
       </c>
       <c r="V26" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="W26" s="2"/>
       <c r="X26" s="2" t="s">
@@ -2590,16 +2595,16 @@
         <v>45</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>66</v>
@@ -2623,7 +2628,7 @@
         <v>122</v>
       </c>
       <c r="V27" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="W27" s="2"/>
       <c r="X27" s="2" t="s">
@@ -2650,7 +2655,7 @@
         <v>6</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="R28" s="1" t="s">
         <v>23</v>
@@ -2665,7 +2670,7 @@
         <v>129</v>
       </c>
       <c r="V28" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="W28" s="2"/>
       <c r="X28" s="2" t="s">
@@ -2680,10 +2685,10 @@
         <v>47</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>70</v>
@@ -2698,7 +2703,7 @@
         <v>4</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="R29" s="1" t="s">
         <v>95</v>
@@ -2713,7 +2718,7 @@
         <v>14</v>
       </c>
       <c r="V29" s="2" t="s">
-        <v>209</v>
+        <v>249</v>
       </c>
       <c r="W29" s="2"/>
       <c r="X29" s="2" t="s">
@@ -2728,17 +2733,17 @@
         <v>48</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="O30" s="3" t="s">
         <v>1</v>
       </c>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="R30" s="4" t="s">
         <v>96</v>
@@ -2753,7 +2758,7 @@
         <v>14</v>
       </c>
       <c r="V30" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="W30" s="2"/>
       <c r="X30" s="4" t="s">
@@ -2768,10 +2773,10 @@
         <v>50</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>65</v>
@@ -2789,7 +2794,7 @@
         <v>51</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="S31" s="2">
         <v>1</v>
@@ -2801,7 +2806,7 @@
         <v>14</v>
       </c>
       <c r="V31" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="W31" s="2"/>
       <c r="X31" s="2" t="s">
@@ -2840,7 +2845,7 @@
         <v>53</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="S32" s="2">
         <v>1</v>
@@ -2852,7 +2857,7 @@
         <v>14</v>
       </c>
       <c r="V32" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="W32" s="2"/>
       <c r="X32" s="2" t="s">
@@ -2876,10 +2881,10 @@
         <v>1</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="S33" s="2">
         <v>2</v>
@@ -2891,7 +2896,7 @@
         <v>0</v>
       </c>
       <c r="V33" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="W33" s="2"/>
       <c r="X33" s="2" t="s">
@@ -2906,7 +2911,7 @@
         <v>55</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>65</v>
@@ -2918,10 +2923,10 @@
         <v>3</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="S34" s="2">
         <v>2</v>
@@ -2933,7 +2938,7 @@
         <v>0</v>
       </c>
       <c r="V34" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="W34" s="2"/>
       <c r="X34" s="2" t="s">
@@ -2948,7 +2953,7 @@
         <v>56</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>66</v>
@@ -2969,10 +2974,10 @@
         <v>7</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="S35" s="2">
         <v>1</v>
@@ -2984,7 +2989,7 @@
         <v>133</v>
       </c>
       <c r="V35" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="W35" s="2"/>
       <c r="X35" s="2" t="s">
@@ -3017,10 +3022,10 @@
         <v>6</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="S36" s="2">
         <v>1</v>
@@ -3032,7 +3037,7 @@
         <v>134</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="W36" s="2"/>
       <c r="X36" s="2" t="s">
@@ -3047,7 +3052,7 @@
         <v>58</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>66</v>
@@ -3068,10 +3073,10 @@
         <v>9</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="S37" s="2">
         <v>1</v>
@@ -3083,7 +3088,7 @@
         <v>130</v>
       </c>
       <c r="V37" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="W37" s="2"/>
       <c r="X37" s="2" t="s">
@@ -3098,7 +3103,7 @@
         <v>59</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>65</v>
@@ -3131,10 +3136,10 @@
         <v>106</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="S38" s="2">
         <v>1</v>
@@ -3146,7 +3151,7 @@
         <v>130</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>208</v>
+        <v>250</v>
       </c>
       <c r="W38" s="2"/>
       <c r="X38" s="2" t="s">
@@ -3161,10 +3166,10 @@
         <v>60</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>70</v>
@@ -3188,10 +3193,10 @@
         <v>8</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="S39" s="2">
         <v>1</v>
@@ -3203,7 +3208,7 @@
         <v>129</v>
       </c>
       <c r="V39" s="2" t="s">
-        <v>211</v>
+        <v>252</v>
       </c>
       <c r="W39" s="2"/>
       <c r="X39" s="2" t="s">
@@ -3218,16 +3223,16 @@
         <v>61</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>251</v>
-      </c>
       <c r="D40" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>66</v>
@@ -3242,10 +3247,10 @@
         <v>7</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="S40" s="2">
         <v>1</v>
@@ -3257,7 +3262,7 @@
         <v>1</v>
       </c>
       <c r="V40" s="2" t="s">
-        <v>214</v>
+        <v>253</v>
       </c>
       <c r="W40" s="2"/>
       <c r="X40" s="2" t="s">
@@ -3272,7 +3277,7 @@
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>66</v>
@@ -3290,7 +3295,7 @@
         <v>9</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="R41" s="2" t="s">
         <v>158</v>
@@ -3305,7 +3310,7 @@
         <v>129</v>
       </c>
       <c r="V41" s="2" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="W41" s="2"/>
       <c r="X41" s="2" t="s">
@@ -3320,10 +3325,10 @@
         <v>63</v>
       </c>
       <c r="F42" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>65</v>
@@ -3332,10 +3337,10 @@
         <v>7</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="S42" s="2">
         <v>2</v>
@@ -3347,7 +3352,7 @@
         <v>14</v>
       </c>
       <c r="V42" s="2" t="s">
-        <v>229</v>
+        <v>254</v>
       </c>
       <c r="W42" s="2"/>
       <c r="X42" s="2" t="s">

</xml_diff>

<commit_message>
add chronology assignment for Chinese phase
</commit_message>
<xml_diff>
--- a/analysis/data/Supplementary_Information/KWL_layer_assign_details.xlsx
+++ b/analysis/data/Supplementary_Information/KWL_layer_assign_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/Supplementary_Information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A890A5-FDD6-204B-819B-3E5FE08B24D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD2985A-B331-F14C-9F3E-D4F64162351B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="460" windowWidth="28300" windowHeight="16540" xr2:uid="{8078604F-F89D-654A-983C-649D14E5F3E8}"/>
+    <workbookView xWindow="980" yWindow="460" windowWidth="28300" windowHeight="16540" xr2:uid="{8078604F-F89D-654A-983C-649D14E5F3E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="292">
   <si>
     <t>L1</t>
   </si>
@@ -308,9 +308,6 @@
     <t>jar*2, stoneware*1</t>
   </si>
   <si>
-    <t>pipe*2</t>
-  </si>
-  <si>
     <t>the earliest layer with diagnostic items</t>
   </si>
   <si>
@@ -335,12 +332,6 @@
     <t>stratigraphic analysis based on field note</t>
   </si>
   <si>
-    <t>pipe*1, jar*1, stoneware*1</t>
-  </si>
-  <si>
-    <t>pipe*4, jar*1</t>
-  </si>
-  <si>
     <t>L7: 418-0 BP,                    L9: 913-737 BP (790),              L13: 1256-1145 BP (1174)</t>
   </si>
   <si>
@@ -731,12 +722,6 @@
     <t>assigning the layer indicating the start of Chinese phase</t>
   </si>
   <si>
-    <t>tile</t>
-  </si>
-  <si>
-    <t>tile, jar*2</t>
-  </si>
-  <si>
     <t>bricks</t>
   </si>
   <si>
@@ -761,21 +746,9 @@
     <t>tiles, bricks</t>
   </si>
   <si>
-    <t>bricks, jar*1</t>
-  </si>
-  <si>
-    <t>tiles, brciks, jar*2</t>
-  </si>
-  <si>
-    <t>tiles, bricks, jar*1, stoneware*1</t>
-  </si>
-  <si>
     <t>tiles, pipe*1, jar*1</t>
   </si>
   <si>
-    <t>Chinese phase indicated by tiles in L1 that continue to L2 according to soil color</t>
-  </si>
-  <si>
     <t>European phase indicated by jar in L3 with the evidence of consistent color, context, and depth with P071 and P085</t>
   </si>
   <si>
@@ -801,6 +774,141 @@
   </si>
   <si>
     <t>Chinese phase indicated by the consistent color, context, and depth of L1 with P040 and P042</t>
+  </si>
+  <si>
+    <t>Lack of Chinese context due to the disturbance in upper layers</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L1 that continue to L2 according to yellowish soil color</t>
+  </si>
+  <si>
+    <t>tiles, plate*1, jar*2</t>
+  </si>
+  <si>
+    <t>plate*1</t>
+  </si>
+  <si>
+    <t>plate*1, jar*1</t>
+  </si>
+  <si>
+    <t>tiles, spoon*1</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by the consistent soil color, context, and depth of L8 with P052 and P064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chinese phase indicated by tiles in L2 and yellowish soil color </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chinese phase indicated by the consistent soil color, context, and depth of L3with P052 </t>
+  </si>
+  <si>
+    <t>bricks, tiles, jar*1</t>
+  </si>
+  <si>
+    <t>bricks, tiles, pipe*1</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L2 that continue to L3 according to yellowish soil color</t>
+  </si>
+  <si>
+    <t>Chinese phase decided based on previous procelain study (Hsieh 2009) indicating high diversity and quantity in L2</t>
+  </si>
+  <si>
+    <t>Chinese phase decided based on previous procelain study (Hsieh 2009) indicating high diversity and quantity in L3 and the presence of tiles</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by the high proportion of tiles starting from L4 and yellowish color</t>
+  </si>
+  <si>
+    <t>tiles, bricks, jar*1</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L3 and previous procelain study (Hsieh 2009) indicating high diversity and quantity in L2-L4</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L2 and previous procelain study (Hsieh 2009) indicating high diversity and quantity in L2-L4</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L3 with previous procelain study (Hsieh 2009) indicating high diversity and quantity</t>
+  </si>
+  <si>
+    <t>jar*1, stoneware*1</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L3 and yellowish soil color</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L1 and the consistent color, context, and depth of L1 with P066</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L1 and previous procelain study (Hsieh 2009) indicating high diversity and quantity in L1</t>
+  </si>
+  <si>
+    <t>Chinese phase decided based on previous procelain study (Hsieh 2009) indicating high diversity and quantity in L2 and the presence of porcelain plate</t>
+  </si>
+  <si>
+    <t>tiles, pipe*2</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L6 and yellowish color</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L5 and the consistent color, context, and depth with P073</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L4 and yellowish color</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L3 and yellowish color</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L2 and the consistent color, context, and depth with P078</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L2 and yellowish color</t>
+  </si>
+  <si>
+    <t>tiles, pipe*1, jar*1, stoneware*1</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L1 and yellowish color</t>
+  </si>
+  <si>
+    <t>tiles, pipe*4, jar*1</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L2 and the consistent color, context, and depth with P083</t>
+  </si>
+  <si>
+    <t>tiles, jar*2, stoneware*1</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles and bricks in L1 and the consistent color, context, and depth with P086</t>
+  </si>
+  <si>
+    <t>tiles, bricks, tiles, jar*1, stoneware*1</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles L4 and yellowish color</t>
+  </si>
+  <si>
+    <t>tiles, plate*1, pipe*1, jar*2</t>
+  </si>
+  <si>
+    <t>Chinese phase decided based on previous procelain study (Hsieh 2009) indicating high diversity and quantity in L1-L2 and the presence of tiles</t>
+  </si>
+  <si>
+    <t>Chinese phase decided based on previous procelain study (Hsieh 2009) indicating high diversity and quantity in L2-L4 and the presence of tiles</t>
+  </si>
+  <si>
+    <t>Chinese phase decided based on previous procelain study (Hsieh 2009) indicating high diversity and quantity in L2-L3 and the presence of tiles</t>
+  </si>
+  <si>
+    <t>Chinese phase decided based on previous procelain study (Hsieh 2009) indicating high diversity and quantity in L2 and the presence of tiles and bricks</t>
+  </si>
+  <si>
+    <t>tiles, bricks, jar*2</t>
   </si>
 </sst>
 </file>
@@ -1179,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B88541E-9DAB-0E45-BDCD-701CF40445C7}">
   <dimension ref="A1:Y42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="106" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1244,37 +1352,37 @@
         <v>12</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="Q1" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="R1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="51" x14ac:dyDescent="0.2">
@@ -1282,7 +1390,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>65</v>
@@ -1300,10 +1408,10 @@
         <v>8</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="S2" s="2">
         <v>1</v>
@@ -1315,10 +1423,10 @@
         <v>14</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>6</v>
@@ -1350,13 +1458,13 @@
         <v>7</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="S3" s="2">
         <v>1</v>
@@ -1368,10 +1476,10 @@
         <v>14</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>4</v>
@@ -1401,7 +1509,7 @@
         <v>49</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="S4" s="4">
         <v>3</v>
@@ -1413,9 +1521,11 @@
         <v>14</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="W4" s="2"/>
+        <v>135</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>247</v>
+      </c>
       <c r="X4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1428,7 +1538,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>65</v>
@@ -1443,13 +1553,13 @@
         <v>11</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="S5" s="2">
         <v>1</v>
@@ -1461,9 +1571,11 @@
         <v>14</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="W5" s="2"/>
+        <v>137</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="X5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1476,10 +1588,10 @@
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>80</v>
@@ -1494,13 +1606,13 @@
         <v>7</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="S6" s="2">
         <v>1</v>
@@ -1512,17 +1624,19 @@
         <v>14</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="W6" s="2"/>
+        <v>142</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>254</v>
+      </c>
       <c r="X6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -1554,10 +1668,10 @@
         <v>11</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="S7" s="2">
         <v>1</v>
@@ -1569,14 +1683,16 @@
         <v>14</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="W7" s="2"/>
+        <v>143</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>255</v>
+      </c>
       <c r="X7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="51" x14ac:dyDescent="0.2">
@@ -1602,10 +1718,10 @@
         <v>5</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="S8" s="2">
         <v>2</v>
@@ -1617,9 +1733,11 @@
         <v>14</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="W8" s="2"/>
+        <v>146</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>247</v>
+      </c>
       <c r="X8" s="2" t="s">
         <v>3</v>
       </c>
@@ -1627,7 +1745,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1644,24 +1762,26 @@
         <v>5</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="S9" s="2">
         <v>1</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="W9" s="2"/>
+        <v>148</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>259</v>
+      </c>
       <c r="X9" s="2" t="s">
         <v>5</v>
       </c>
@@ -1669,12 +1789,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>66</v>
+        <v>232</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>65</v>
@@ -1689,7 +1809,7 @@
         <v>6</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>23</v>
@@ -1698,15 +1818,17 @@
         <v>1</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="W10" s="2"/>
+        <v>149</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>258</v>
+      </c>
       <c r="X10" s="2" t="s">
         <v>6</v>
       </c>
@@ -1714,10 +1836,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D11" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="F11" s="1" t="s">
         <v>79</v>
       </c>
@@ -1743,21 +1871,23 @@
         <v>25</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="S11" s="2">
         <v>1</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="W11" s="2"/>
+        <v>151</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>260</v>
+      </c>
       <c r="X11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1765,18 +1895,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>66</v>
@@ -1800,24 +1933,26 @@
         <v>9</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="S12" s="2">
         <v>1</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="W12" s="2"/>
+        <v>153</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="X12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1830,16 +1965,16 @@
         <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>73</v>
@@ -1860,24 +1995,26 @@
         <v>9</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="S13" s="2">
         <v>1</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="W13" s="2"/>
+        <v>154</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="X13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1885,15 +2022,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="C14" s="1" t="s">
-        <v>66</v>
+        <v>262</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>70</v>
@@ -1917,27 +2057,29 @@
         <v>11</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>29</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="S14" s="2">
         <v>1</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="W14" s="2"/>
+        <v>156</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>263</v>
+      </c>
       <c r="X14" s="2" t="s">
         <v>8</v>
       </c>
@@ -1945,12 +2087,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>70</v>
@@ -1977,24 +2122,26 @@
         <v>12</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="S15" s="2">
         <v>1</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="W15" s="2"/>
+        <v>157</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>264</v>
+      </c>
       <c r="X15" s="2" t="s">
         <v>8</v>
       </c>
@@ -2002,21 +2149,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>66</v>
@@ -2028,7 +2178,7 @@
         <v>43</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="S16" s="2">
         <v>1</v>
@@ -2040,9 +2190,11 @@
         <v>2</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="W16" s="2"/>
+        <v>160</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>265</v>
+      </c>
       <c r="X16" s="2" t="s">
         <v>4</v>
       </c>
@@ -2055,19 +2207,22 @@
         <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>238</v>
+        <v>266</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>66</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>77</v>
@@ -2085,27 +2240,29 @@
         <v>11</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="S17" s="2">
         <v>1</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="U17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="W17" s="2"/>
+        <v>162</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>267</v>
+      </c>
       <c r="X17" s="2" t="s">
         <v>6</v>
       </c>
@@ -2118,10 +2275,10 @@
         <v>33</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>66</v>
+        <v>251</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>65</v>
@@ -2130,7 +2287,7 @@
         <v>4</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="R18" s="1" t="s">
         <v>34</v>
@@ -2139,15 +2296,17 @@
         <v>1</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="W18" s="2"/>
+        <v>163</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>268</v>
+      </c>
       <c r="X18" s="2" t="s">
         <v>3</v>
       </c>
@@ -2160,7 +2319,7 @@
         <v>35</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>66</v>
@@ -2169,13 +2328,13 @@
         <v>2</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="Q19" s="2" t="s">
         <v>36</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="S19" s="2">
         <v>1</v>
@@ -2187,9 +2346,11 @@
         <v>0</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="W19" s="2"/>
+        <v>238</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>269</v>
+      </c>
       <c r="X19" s="2" t="s">
         <v>2</v>
       </c>
@@ -2197,10 +2358,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="B20" s="7" t="s">
+        <v>250</v>
+      </c>
       <c r="D20" s="1" t="s">
         <v>66</v>
       </c>
@@ -2223,24 +2387,26 @@
         <v>9</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="S20" s="2">
         <v>1</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="U20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="W20" s="2"/>
+        <v>166</v>
+      </c>
+      <c r="W20" s="2" t="s">
+        <v>270</v>
+      </c>
       <c r="X20" s="2" t="s">
         <v>5</v>
       </c>
@@ -2253,19 +2419,22 @@
         <v>38</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>230</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>65</v>
+        <v>234</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>91</v>
+        <v>271</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>91</v>
+        <v>271</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>67</v>
+        <v>237</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>67</v>
@@ -2280,24 +2449,26 @@
         <v>9</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S21" s="2">
         <v>1</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="W21" s="2"/>
+        <v>167</v>
+      </c>
+      <c r="W21" s="2" t="s">
+        <v>272</v>
+      </c>
       <c r="X21" s="2" t="s">
         <v>9</v>
       </c>
@@ -2310,19 +2481,19 @@
         <v>39</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>74</v>
@@ -2343,10 +2514,10 @@
         <v>12</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="S22" s="2">
         <v>1</v>
@@ -2355,12 +2526,14 @@
         <v>9</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="W22" s="2"/>
+        <v>168</v>
+      </c>
+      <c r="W22" s="2" t="s">
+        <v>272</v>
+      </c>
       <c r="X22" s="2" t="s">
         <v>10</v>
       </c>
@@ -2368,24 +2541,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>65</v>
@@ -2412,24 +2585,26 @@
         <v>11</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S23" s="2">
         <v>1</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="W23" s="2"/>
+        <v>169</v>
+      </c>
+      <c r="W23" s="2" t="s">
+        <v>273</v>
+      </c>
       <c r="X23" s="2" t="s">
         <v>8</v>
       </c>
@@ -2437,18 +2612,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="51" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>235</v>
+        <v>252</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>66</v>
@@ -2457,24 +2632,26 @@
         <v>7</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="S24" s="2">
         <v>1</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="W24" s="2"/>
+        <v>239</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>260</v>
+      </c>
       <c r="X24" s="2" t="s">
         <v>7</v>
       </c>
@@ -2482,24 +2659,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="51" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>237</v>
+        <v>256</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>66</v>
@@ -2514,24 +2691,26 @@
         <v>10</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="S25" s="2">
         <v>1</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="W25" s="2"/>
+        <v>242</v>
+      </c>
+      <c r="W25" s="2" t="s">
+        <v>260</v>
+      </c>
       <c r="X25" s="2" t="s">
         <v>5</v>
       </c>
@@ -2544,16 +2723,16 @@
         <v>44</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>66</v>
@@ -2565,10 +2744,10 @@
         <v>5</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="S26" s="2">
         <v>1</v>
@@ -2577,12 +2756,14 @@
         <v>4</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="V26" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="W26" s="2"/>
+        <v>178</v>
+      </c>
+      <c r="W26" s="2" t="s">
+        <v>260</v>
+      </c>
       <c r="X26" s="2" t="s">
         <v>4</v>
       </c>
@@ -2595,16 +2776,16 @@
         <v>45</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>66</v>
@@ -2613,7 +2794,7 @@
         <v>6</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R27" s="1" t="s">
         <v>23</v>
@@ -2625,12 +2806,14 @@
         <v>6</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="V27" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="W27" s="2"/>
+        <v>181</v>
+      </c>
+      <c r="W27" s="2" t="s">
+        <v>274</v>
+      </c>
       <c r="X27" s="2" t="s">
         <v>6</v>
       </c>
@@ -2642,8 +2825,14 @@
       <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="B28" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>230</v>
+      </c>
       <c r="D28" s="1" t="s">
-        <v>66</v>
+        <v>232</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>66</v>
@@ -2655,7 +2844,7 @@
         <v>6</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="R28" s="1" t="s">
         <v>23</v>
@@ -2664,15 +2853,17 @@
         <v>1</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="V28" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="W28" s="2"/>
+        <v>181</v>
+      </c>
+      <c r="W28" s="2" t="s">
+        <v>275</v>
+      </c>
       <c r="X28" s="2" t="s">
         <v>6</v>
       </c>
@@ -2685,13 +2876,13 @@
         <v>47</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>69</v>
@@ -2703,24 +2894,26 @@
         <v>4</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S29" s="2">
         <v>1</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="V29" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="W29" s="2"/>
+        <v>240</v>
+      </c>
+      <c r="W29" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="X29" s="2" t="s">
         <v>4</v>
       </c>
@@ -2733,20 +2926,20 @@
         <v>48</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>240</v>
       </c>
       <c r="O30" s="3" t="s">
         <v>1</v>
       </c>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="R30" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S30" s="4">
         <v>3</v>
@@ -2758,9 +2951,11 @@
         <v>14</v>
       </c>
       <c r="V30" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="W30" s="2"/>
+        <v>183</v>
+      </c>
+      <c r="W30" s="2" t="s">
+        <v>247</v>
+      </c>
       <c r="X30" s="4" t="s">
         <v>1</v>
       </c>
@@ -2773,10 +2968,10 @@
         <v>50</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>65</v>
@@ -2794,7 +2989,7 @@
         <v>51</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="S31" s="2">
         <v>1</v>
@@ -2806,9 +3001,11 @@
         <v>14</v>
       </c>
       <c r="V31" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="W31" s="2"/>
+        <v>186</v>
+      </c>
+      <c r="W31" s="2" t="s">
+        <v>277</v>
+      </c>
       <c r="X31" s="2" t="s">
         <v>3</v>
       </c>
@@ -2821,7 +3018,7 @@
         <v>52</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>100</v>
+        <v>278</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>66</v>
@@ -2845,7 +3042,7 @@
         <v>53</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="S32" s="2">
         <v>1</v>
@@ -2857,9 +3054,11 @@
         <v>14</v>
       </c>
       <c r="V32" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="W32" s="2"/>
+        <v>187</v>
+      </c>
+      <c r="W32" s="2" t="s">
+        <v>279</v>
+      </c>
       <c r="X32" s="2" t="s">
         <v>2</v>
       </c>
@@ -2872,19 +3071,19 @@
         <v>54</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>66</v>
+        <v>232</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>101</v>
+        <v>280</v>
       </c>
       <c r="O33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="S33" s="2">
         <v>2</v>
@@ -2896,9 +3095,11 @@
         <v>0</v>
       </c>
       <c r="V33" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="W33" s="2"/>
+        <v>188</v>
+      </c>
+      <c r="W33" s="2" t="s">
+        <v>281</v>
+      </c>
       <c r="X33" s="2" t="s">
         <v>1</v>
       </c>
@@ -2911,7 +3112,10 @@
         <v>55</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>65</v>
@@ -2923,10 +3127,10 @@
         <v>3</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="S34" s="2">
         <v>2</v>
@@ -2938,9 +3142,11 @@
         <v>0</v>
       </c>
       <c r="V34" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="W34" s="2"/>
+        <v>193</v>
+      </c>
+      <c r="W34" s="2" t="s">
+        <v>283</v>
+      </c>
       <c r="X34" s="2" t="s">
         <v>1</v>
       </c>
@@ -2948,18 +3154,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="51" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>66</v>
+        <v>232</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>90</v>
+        <v>282</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>85</v>
@@ -2974,24 +3183,26 @@
         <v>7</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S35" s="2">
         <v>1</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U35" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="V35" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="W35" s="2"/>
+        <v>195</v>
+      </c>
+      <c r="W35" s="2" t="s">
+        <v>287</v>
+      </c>
       <c r="X35" s="2" t="s">
         <v>4</v>
       </c>
@@ -3004,7 +3215,10 @@
         <v>57</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>65</v>
+        <v>234</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>66</v>
@@ -3022,10 +3236,10 @@
         <v>6</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="S36" s="2">
         <v>1</v>
@@ -3034,12 +3248,14 @@
         <v>5</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="W36" s="2"/>
+        <v>198</v>
+      </c>
+      <c r="W36" s="2" t="s">
+        <v>277</v>
+      </c>
       <c r="X36" s="2" t="s">
         <v>5</v>
       </c>
@@ -3051,8 +3267,14 @@
       <c r="A37" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="C37" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="D37" s="1" t="s">
-        <v>238</v>
+        <v>284</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>66</v>
@@ -3073,24 +3295,26 @@
         <v>9</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="S37" s="2">
         <v>1</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="U37" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="V37" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="W37" s="2"/>
+        <v>199</v>
+      </c>
+      <c r="W37" s="2" t="s">
+        <v>285</v>
+      </c>
       <c r="X37" s="2" t="s">
         <v>7</v>
       </c>
@@ -3103,13 +3327,13 @@
         <v>59</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>65</v>
+        <v>234</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>66</v>
+        <v>232</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>70</v>
@@ -3133,13 +3357,13 @@
         <v>11</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="S38" s="2">
         <v>1</v>
@@ -3148,12 +3372,14 @@
         <v>7</v>
       </c>
       <c r="U38" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="W38" s="2"/>
+        <v>241</v>
+      </c>
+      <c r="W38" s="2" t="s">
+        <v>288</v>
+      </c>
       <c r="X38" s="2" t="s">
         <v>8</v>
       </c>
@@ -3161,21 +3387,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="51" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>70</v>
+        <v>235</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>71</v>
+        <v>286</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>72</v>
@@ -3193,24 +3419,26 @@
         <v>8</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="S39" s="2">
         <v>1</v>
       </c>
       <c r="T39" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="V39" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="W39" s="2"/>
+        <v>243</v>
+      </c>
+      <c r="W39" s="2" t="s">
+        <v>289</v>
+      </c>
       <c r="X39" s="2" t="s">
         <v>6</v>
       </c>
@@ -3223,16 +3451,16 @@
         <v>61</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>243</v>
+        <v>291</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>66</v>
@@ -3247,24 +3475,26 @@
         <v>7</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="S40" s="2">
         <v>1</v>
       </c>
       <c r="T40" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="U40" s="1" t="s">
         <v>1</v>
       </c>
       <c r="V40" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="W40" s="2"/>
+        <v>244</v>
+      </c>
+      <c r="W40" s="2" t="s">
+        <v>290</v>
+      </c>
       <c r="X40" s="2" t="s">
         <v>5</v>
       </c>
@@ -3272,12 +3502,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>66</v>
@@ -3295,24 +3528,26 @@
         <v>9</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="S41" s="2">
         <v>1</v>
       </c>
       <c r="T41" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="U41" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="V41" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="W41" s="2"/>
+        <v>216</v>
+      </c>
+      <c r="W41" s="2" t="s">
+        <v>289</v>
+      </c>
       <c r="X41" s="2" t="s">
         <v>6</v>
       </c>
@@ -3325,10 +3560,10 @@
         <v>63</v>
       </c>
       <c r="F42" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>65</v>
@@ -3337,10 +3572,10 @@
         <v>7</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="S42" s="2">
         <v>2</v>
@@ -3352,9 +3587,11 @@
         <v>14</v>
       </c>
       <c r="V42" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="W42" s="2"/>
+        <v>245</v>
+      </c>
+      <c r="W42" s="2" t="s">
+        <v>247</v>
+      </c>
       <c r="X42" s="2" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
fix typos in spreadsheet
</commit_message>
<xml_diff>
--- a/analysis/data/Supplementary_Information/KWL_layer_assign_details.xlsx
+++ b/analysis/data/Supplementary_Information/KWL_layer_assign_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/Supplementary_Information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD2985A-B331-F14C-9F3E-D4F64162351B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87F708F-5113-9C4A-9054-9ECB7EB6456D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="460" windowWidth="28300" windowHeight="16540" xr2:uid="{8078604F-F89D-654A-983C-649D14E5F3E8}"/>
   </bookViews>
@@ -122,9 +122,6 @@
     <t>P063</t>
   </si>
   <si>
-    <t>natural depression showing on cross section, more potsheds from L7</t>
-  </si>
-  <si>
     <t>P064</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>P070</t>
   </si>
   <si>
-    <t>more feautres and charcolas in L3</t>
-  </si>
-  <si>
     <t>P071</t>
   </si>
   <si>
@@ -371,9 +365,6 @@
     <t>color change in L5 and more potsherds in L7</t>
   </si>
   <si>
-    <t>European phase indicated by Anping jar in L7 accompied with more potsherds</t>
-  </si>
-  <si>
     <t>L5, L6</t>
   </si>
   <si>
@@ -437,36 +428,15 @@
     <t>big pieces of jar in L2, L3, disturbed to 0 cm</t>
   </si>
   <si>
-    <t>European phase indicated by more pieces of Anping jars in L5 with the references of more potsherds and radiocarbon date</t>
-  </si>
-  <si>
     <t>European phase indicated by more pieces of Anping jars and pipe in L1 with the references of connection with P041</t>
   </si>
   <si>
-    <t>more artifacts and charcols in L10-L11</t>
-  </si>
-  <si>
     <t>European phase indicated by more pieces of Anping jars and pipe in L11</t>
   </si>
   <si>
-    <t xml:space="preserve">C14 dates seem not very reasonable indicating distrubance or camtamination of samples. Small pieces of jar in L12, , likely postdepositional disturbance </t>
-  </si>
-  <si>
-    <t>burial date contradicts other rediocarbon dates, possibly old wood effect or a alluvial layer</t>
-  </si>
-  <si>
     <t>increasing charcoals and potsherds beginning from L6, color changes to darker in L8</t>
   </si>
   <si>
-    <t>color changes in L8 with a wide vaireity of artifacts</t>
-  </si>
-  <si>
-    <t>European phase indicated by Anping jars and colar change in L8 with the referrence of radiocarbon date of L7</t>
-  </si>
-  <si>
-    <t>European phase indicated by Anping jars and colar change in L8</t>
-  </si>
-  <si>
     <t xml:space="preserve">pieces of jar in L5-16, likely postdepositional disturbance </t>
   </si>
   <si>
@@ -509,9 +479,6 @@
     <t>European phase indicated by jars and pipes in L9 with color change</t>
   </si>
   <si>
-    <t>More pots, charcols, and a wide variety of artifacts starting from L9, color is darker</t>
-  </si>
-  <si>
     <t>small pieces in L7 &lt; 10g, likely postdepositional disturbance</t>
   </si>
   <si>
@@ -521,12 +488,6 @@
     <t xml:space="preserve">more charcoals and local potsherds starting from L7, color turns to more black </t>
   </si>
   <si>
-    <t xml:space="preserve">European phase indicated by the consistent color, context, and depth of L7 with adjecent units, although no direct dignostic artifacts found </t>
-  </si>
-  <si>
-    <t xml:space="preserve">European phase indicated by the consistent color, context, and depth of L4 with adjecent units, although no direct dignostic artifacts found </t>
-  </si>
-  <si>
     <t>not many jars, L3 is 20 cm thick</t>
   </si>
   <si>
@@ -551,9 +512,6 @@
     <t>river on section c, pieces of jars in L12 and 13 &gt; 80g at B section coming from midden</t>
   </si>
   <si>
-    <t>more potsherds and charcols in L9 with darker soil color</t>
-  </si>
-  <si>
     <t>charcoals and potsherds in L9 and L10 with darker soil color</t>
   </si>
   <si>
@@ -572,9 +530,6 @@
     <t>European phase indicated by jar in L5 with darker soil color</t>
   </si>
   <si>
-    <t>more potsherds and charcols in L5, darker soil color</t>
-  </si>
-  <si>
     <t>jar pieces in L6 &lt; 10g, likely postdepositional disturbance. The top of L6 might relate to L5, but it is 20cm thick so excluded</t>
   </si>
   <si>
@@ -584,9 +539,6 @@
     <t>more potsherds in L6-L7</t>
   </si>
   <si>
-    <t>European phase indicated by highr proportion of jar in L2 with darker soil color</t>
-  </si>
-  <si>
     <t>more potsherds in L1-L2, darker soil color</t>
   </si>
   <si>
@@ -596,12 +548,6 @@
     <t>European phase indicated by jar in L4 with darker color</t>
   </si>
   <si>
-    <t>European phase indicated by highr proportion of jar, pipe, and stoneware in L3</t>
-  </si>
-  <si>
-    <t>European phase indicated by highr proportion of pipes, and jar in L2 with darker color</t>
-  </si>
-  <si>
     <t>more charcoals and trade beads in L2, darker soil color</t>
   </si>
   <si>
@@ -614,18 +560,9 @@
     <t>only pipe stems, L2 is 20cm thick</t>
   </si>
   <si>
-    <t xml:space="preserve">European phase indicated by the consistent color, context, and depth of L2 with adjecent units, although no direct dignostic artifacts found </t>
-  </si>
-  <si>
     <t>jars in L7 &lt; 30g and L8 &lt; 70g, likely coming from midden</t>
   </si>
   <si>
-    <t>European phase indicated by highr proportion of jar and stoneware in L5 with dark soil color</t>
-  </si>
-  <si>
-    <t>more potsherds and charcols in L5-L6</t>
-  </si>
-  <si>
     <t xml:space="preserve">jar pieces in L7 &lt; 10g, likely postdepositional disturbance </t>
   </si>
   <si>
@@ -650,12 +587,6 @@
     <t>jar pieces in L8 &lt; 10g, likely postdepositional disturbance, and pieces in L7 might come from midden</t>
   </si>
   <si>
-    <t>more potsherds and charcols in L5-L6, darker soil color</t>
-  </si>
-  <si>
-    <t>more charcols and potsherds in L4-L5, darker soil color</t>
-  </si>
-  <si>
     <t>black color in L4-L5 observed on west wall</t>
   </si>
   <si>
@@ -683,9 +614,6 @@
     <t>more charcoals and local potsherds in L6-L7 with color change</t>
   </si>
   <si>
-    <t>European phase indicated by highr proportion of jar in L7 with dark soil color</t>
-  </si>
-  <si>
     <t>more local potsherds in L6-L7</t>
   </si>
   <si>
@@ -695,9 +623,6 @@
     <t>one piece of jar in L6 &gt; 120g, likely postdepositional disturbance</t>
   </si>
   <si>
-    <t>C14 dates seem not very reasonable indicating distrubance or camtamination of samples, pieces of jar in L11, likely coming from features</t>
-  </si>
-  <si>
     <t xml:space="preserve">small jar pieces in L7 &lt; 10g, likely postdepositional disturbance </t>
   </si>
   <si>
@@ -749,9 +674,6 @@
     <t>tiles, pipe*1, jar*1</t>
   </si>
   <si>
-    <t>European phase indicated by jar in L3 with the evidence of consistent color, context, and depth with P071 and P085</t>
-  </si>
-  <si>
     <t>European phase indicated by jar in L8 with the evidence of consistent color, context, and depth with P062</t>
   </si>
   <si>
@@ -767,9 +689,6 @@
     <t>European phase indicated by jar in L7 with the evidence of consistent color, artifacts, and depth with P075</t>
   </si>
   <si>
-    <t xml:space="preserve">European phase indicated by the consistent color, context, and depth of L6 with P092, although no direct dignostic artifacts found </t>
-  </si>
-  <si>
     <t>European phase indicated by jar in L5 with the evidence of consistent color, and depth with P092 and P078</t>
   </si>
   <si>
@@ -812,27 +731,12 @@
     <t>Chinese phase indicated by tiles in L2 that continue to L3 according to yellowish soil color</t>
   </si>
   <si>
-    <t>Chinese phase decided based on previous procelain study (Hsieh 2009) indicating high diversity and quantity in L2</t>
-  </si>
-  <si>
-    <t>Chinese phase decided based on previous procelain study (Hsieh 2009) indicating high diversity and quantity in L3 and the presence of tiles</t>
-  </si>
-  <si>
     <t>Chinese phase indicated by the high proportion of tiles starting from L4 and yellowish color</t>
   </si>
   <si>
     <t>tiles, bricks, jar*1</t>
   </si>
   <si>
-    <t>Chinese phase indicated by tiles in L3 and previous procelain study (Hsieh 2009) indicating high diversity and quantity in L2-L4</t>
-  </si>
-  <si>
-    <t>Chinese phase indicated by tiles in L2 and previous procelain study (Hsieh 2009) indicating high diversity and quantity in L2-L4</t>
-  </si>
-  <si>
-    <t>Chinese phase indicated by tiles in L3 with previous procelain study (Hsieh 2009) indicating high diversity and quantity</t>
-  </si>
-  <si>
     <t>jar*1, stoneware*1</t>
   </si>
   <si>
@@ -842,12 +746,6 @@
     <t>Chinese phase indicated by tiles in L1 and the consistent color, context, and depth of L1 with P066</t>
   </si>
   <si>
-    <t>Chinese phase indicated by tiles in L1 and previous procelain study (Hsieh 2009) indicating high diversity and quantity in L1</t>
-  </si>
-  <si>
-    <t>Chinese phase decided based on previous procelain study (Hsieh 2009) indicating high diversity and quantity in L2 and the presence of porcelain plate</t>
-  </si>
-  <si>
     <t>tiles, pipe*2</t>
   </si>
   <si>
@@ -896,19 +794,121 @@
     <t>tiles, plate*1, pipe*1, jar*2</t>
   </si>
   <si>
-    <t>Chinese phase decided based on previous procelain study (Hsieh 2009) indicating high diversity and quantity in L1-L2 and the presence of tiles</t>
-  </si>
-  <si>
-    <t>Chinese phase decided based on previous procelain study (Hsieh 2009) indicating high diversity and quantity in L2-L4 and the presence of tiles</t>
-  </si>
-  <si>
-    <t>Chinese phase decided based on previous procelain study (Hsieh 2009) indicating high diversity and quantity in L2-L3 and the presence of tiles</t>
-  </si>
-  <si>
-    <t>Chinese phase decided based on previous procelain study (Hsieh 2009) indicating high diversity and quantity in L2 and the presence of tiles and bricks</t>
-  </si>
-  <si>
     <t>tiles, bricks, jar*2</t>
+  </si>
+  <si>
+    <t>European phase indicated by Anping jar in L7 accompanied with more potsherds</t>
+  </si>
+  <si>
+    <t>more artifacts and charcoals in L10-L11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C14 dates seem not very reasonable indicating disturbance or contamination of samples. Small pieces of jar in L12, , likely postdepositional disturbance </t>
+  </si>
+  <si>
+    <t>European phase indicated by Anping jars and color change in L8 with the reference of radiocarbon date of L7</t>
+  </si>
+  <si>
+    <t>color changes in L8 with a wide variety of artifacts</t>
+  </si>
+  <si>
+    <t>European phase indicated by Anping jars and color change in L8</t>
+  </si>
+  <si>
+    <t>Chinese phase decided based on previous porcelain study (Hsieh 2009) indicating high diversity and quantity in L2</t>
+  </si>
+  <si>
+    <t>Chinese phase decided based on previous porcelain study (Hsieh 2009) indicating high diversity and quantity in L3 and the presence of tiles</t>
+  </si>
+  <si>
+    <t>natural depression showing on cross section, more potsherds from L7</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L3 and previous porcelain study (Hsieh 2009) indicating high diversity and quantity in L2-L4</t>
+  </si>
+  <si>
+    <t>More pots, charcoals, and a wide variety of artifacts starting from L9, color is darker</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L2 and previous porcelain study (Hsieh 2009) indicating high diversity and quantity in L2-L4</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L3 with previous porcelain study (Hsieh 2009) indicating high diversity and quantity</t>
+  </si>
+  <si>
+    <t>more features and charcoals in L3</t>
+  </si>
+  <si>
+    <t>Chinese phase indicated by tiles in L1 and previous porcelain study (Hsieh 2009) indicating high diversity and quantity in L1</t>
+  </si>
+  <si>
+    <t>Chinese phase decided based on previous porcelain study (Hsieh 2009) indicating high diversity and quantity in L2 and the presence of porcelain plate</t>
+  </si>
+  <si>
+    <t>more potsherds and charcoals in L9 with darker soil color</t>
+  </si>
+  <si>
+    <t>more potsherds and charcoals in L5, darker soil color</t>
+  </si>
+  <si>
+    <t>European phase indicated by higher proportion of jar in L2 with darker soil color</t>
+  </si>
+  <si>
+    <t>European phase indicated by higher proportion of jar, pipe, and stoneware in L3</t>
+  </si>
+  <si>
+    <t>European phase indicated by higher proportion of pipes, and jar in L2 with darker color</t>
+  </si>
+  <si>
+    <t>more charcoals and potsherds in L4-L5, darker soil color</t>
+  </si>
+  <si>
+    <t>European phase indicated by higher proportion of jar and stoneware in L5 with dark soil color</t>
+  </si>
+  <si>
+    <t>Chinese phase decided based on previous porcelain study (Hsieh 2009) indicating high diversity and quantity in L1-L2 and the presence of tiles</t>
+  </si>
+  <si>
+    <t>more potsherds and charcoals in L5-L6, darker soil color</t>
+  </si>
+  <si>
+    <t>C14 dates seem not very reasonable indicating disturbance or contamination of samples, pieces of jar in L11, likely coming from features</t>
+  </si>
+  <si>
+    <t>Chinese phase decided based on previous porcelain study (Hsieh 2009) indicating high diversity and quantity in L2-L4 and the presence of tiles</t>
+  </si>
+  <si>
+    <t>Chinese phase decided based on previous porcelain study (Hsieh 2009) indicating high diversity and quantity in L2-L3 and the presence of tiles</t>
+  </si>
+  <si>
+    <t>more potsherds and charcoals in L5-L6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">European phase indicated by the consistent color, context, and depth of L6 with P092, although no direct diagnostic artifacts found </t>
+  </si>
+  <si>
+    <t>Chinese phase decided based on previous porcelain study (Hsieh 2009) indicating high diversity and quantity in L2 and the presence of tiles and bricks</t>
+  </si>
+  <si>
+    <t>European phase indicated by higher proportion of jar in L7 with dark soil color</t>
+  </si>
+  <si>
+    <t>burial date contradicts other radiocarbon dates, possibly old wood effect or a alluvial layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">European phase indicated by the consistent color, context, and depth of L7 with P065, although no direct diagnostic artifacts found </t>
+  </si>
+  <si>
+    <t xml:space="preserve">European phase indicated by the consistent color, context, and depth of L4 with P080, although no direct diagnostic artifacts found </t>
+  </si>
+  <si>
+    <t>European phase indicated by jar in L3 with the evidence of consistent color, context, and depth with P071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">European phase indicated by the consistent color, context, and depth of L2 with P084 and P086, although no direct diagnostic artifacts found </t>
+  </si>
+  <si>
+    <t>European phase indicated by more pieces of Anping jars in L5 with the references of more potsherds and radiocarbon dates</t>
   </si>
 </sst>
 </file>
@@ -1287,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B88541E-9DAB-0E45-BDCD-701CF40445C7}">
   <dimension ref="A1:Y42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="106" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1310,7 +1310,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1352,37 +1352,37 @@
         <v>12</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="R1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="Y1" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="51" x14ac:dyDescent="0.2">
@@ -1390,28 +1390,28 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="S2" s="2">
         <v>1</v>
@@ -1423,10 +1423,10 @@
         <v>14</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>112</v>
+        <v>254</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>248</v>
+        <v>221</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>6</v>
@@ -1440,31 +1440,31 @@
         <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>221</v>
+        <v>196</v>
       </c>
       <c r="S3" s="2">
         <v>1</v>
@@ -1476,10 +1476,10 @@
         <v>14</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>134</v>
+        <v>291</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>246</v>
+        <v>219</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>4</v>
@@ -1493,23 +1493,23 @@
         <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="S4" s="4">
         <v>3</v>
@@ -1521,10 +1521,10 @@
         <v>14</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>247</v>
+        <v>220</v>
       </c>
       <c r="X4" s="4" t="s">
         <v>0</v>
@@ -1538,28 +1538,28 @@
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>136</v>
+        <v>255</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>138</v>
+        <v>256</v>
       </c>
       <c r="S5" s="2">
         <v>1</v>
@@ -1571,10 +1571,10 @@
         <v>14</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>253</v>
+        <v>226</v>
       </c>
       <c r="X5" s="2" t="s">
         <v>10</v>
@@ -1588,31 +1588,31 @@
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>139</v>
+        <v>286</v>
       </c>
       <c r="S6" s="2">
         <v>1</v>
@@ -1624,10 +1624,10 @@
         <v>14</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>142</v>
+        <v>257</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>254</v>
+        <v>227</v>
       </c>
       <c r="X6" s="2" t="s">
         <v>7</v>
@@ -1641,37 +1641,37 @@
         <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>141</v>
+        <v>258</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="S7" s="2">
         <v>1</v>
@@ -1683,10 +1683,10 @@
         <v>14</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>143</v>
+        <v>259</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>255</v>
+        <v>228</v>
       </c>
       <c r="X7" s="2" t="s">
         <v>7</v>
@@ -1700,28 +1700,28 @@
         <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="S8" s="2">
         <v>2</v>
@@ -1733,10 +1733,10 @@
         <v>14</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>247</v>
+        <v>220</v>
       </c>
       <c r="X8" s="2" t="s">
         <v>3</v>
@@ -1750,37 +1750,37 @@
         <v>21</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="S9" s="2">
         <v>1</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="X9" s="2" t="s">
         <v>5</v>
@@ -1794,22 +1794,22 @@
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>23</v>
@@ -1818,16 +1818,16 @@
         <v>1</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>258</v>
+        <v>231</v>
       </c>
       <c r="X10" s="2" t="s">
         <v>6</v>
@@ -1841,25 +1841,25 @@
         <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N11" s="1">
         <v>1</v>
@@ -1871,22 +1871,22 @@
         <v>25</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="S11" s="2">
         <v>1</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="X11" s="2" t="s">
         <v>7</v>
@@ -1900,58 +1900,58 @@
         <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="S12" s="2">
         <v>1</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>261</v>
+        <v>232</v>
       </c>
       <c r="X12" s="2" t="s">
         <v>8</v>
@@ -1965,55 +1965,55 @@
         <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="S13" s="2">
         <v>1</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>261</v>
+        <v>232</v>
       </c>
       <c r="X13" s="2" t="s">
         <v>8</v>
@@ -2027,55 +2027,55 @@
         <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>262</v>
+        <v>233</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>29</v>
+        <v>262</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="S14" s="2">
         <v>1</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="W14" s="2" t="s">
         <v>263</v>
@@ -2089,31 +2089,31 @@
     </row>
     <row r="15" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="L15" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N15" s="1">
         <v>1</v>
@@ -2122,25 +2122,25 @@
         <v>12</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>158</v>
+        <v>264</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="S15" s="2">
         <v>1</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="X15" s="2" t="s">
         <v>8</v>
@@ -2151,34 +2151,34 @@
     </row>
     <row r="16" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="S16" s="2">
         <v>1</v>
@@ -2190,10 +2190,10 @@
         <v>2</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="X16" s="2" t="s">
         <v>4</v>
@@ -2204,64 +2204,64 @@
     </row>
     <row r="17" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>266</v>
+        <v>234</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="S17" s="2">
         <v>1</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="U17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>162</v>
+        <v>287</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>267</v>
+        <v>235</v>
       </c>
       <c r="X17" s="2" t="s">
         <v>6</v>
@@ -2272,40 +2272,40 @@
     </row>
     <row r="18" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>251</v>
+        <v>224</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>4</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S18" s="2">
         <v>1</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>163</v>
+        <v>288</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>268</v>
+        <v>236</v>
       </c>
       <c r="X18" s="2" t="s">
         <v>3</v>
@@ -2316,25 +2316,25 @@
     </row>
     <row r="19" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>36</v>
+        <v>267</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="S19" s="2">
         <v>1</v>
@@ -2346,10 +2346,10 @@
         <v>0</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>238</v>
+        <v>289</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="X19" s="2" t="s">
         <v>2</v>
@@ -2360,52 +2360,52 @@
     </row>
     <row r="20" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="S20" s="2">
         <v>1</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="U20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="X20" s="2" t="s">
         <v>5</v>
@@ -2416,58 +2416,58 @@
     </row>
     <row r="21" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>271</v>
+        <v>237</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>271</v>
+        <v>237</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>9</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="S21" s="2">
         <v>1</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>272</v>
+        <v>238</v>
       </c>
       <c r="X21" s="2" t="s">
         <v>9</v>
@@ -2478,46 +2478,46 @@
     </row>
     <row r="22" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="S22" s="2">
         <v>1</v>
@@ -2526,13 +2526,13 @@
         <v>9</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>272</v>
+        <v>238</v>
       </c>
       <c r="X22" s="2" t="s">
         <v>10</v>
@@ -2543,67 +2543,67 @@
     </row>
     <row r="23" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>172</v>
+        <v>270</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="S23" s="2">
         <v>1</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>273</v>
+        <v>239</v>
       </c>
       <c r="X23" s="2" t="s">
         <v>8</v>
@@ -2614,43 +2614,43 @@
     </row>
     <row r="24" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>252</v>
+        <v>225</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="S24" s="2">
         <v>1</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>239</v>
+        <v>213</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="X24" s="2" t="s">
         <v>7</v>
@@ -2661,55 +2661,55 @@
     </row>
     <row r="25" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>256</v>
+        <v>229</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>10</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="S25" s="2">
         <v>1</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="X25" s="2" t="s">
         <v>5</v>
@@ -2720,34 +2720,34 @@
     </row>
     <row r="26" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>179</v>
+        <v>271</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="S26" s="2">
         <v>1</v>
@@ -2756,13 +2756,13 @@
         <v>4</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="V26" s="2" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="X26" s="2" t="s">
         <v>4</v>
@@ -2773,28 +2773,28 @@
     </row>
     <row r="27" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>257</v>
-      </c>
       <c r="D27" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="R27" s="1" t="s">
         <v>23</v>
@@ -2806,13 +2806,13 @@
         <v>6</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="V27" s="2" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="W27" s="2" t="s">
-        <v>274</v>
+        <v>240</v>
       </c>
       <c r="X27" s="2" t="s">
         <v>6</v>
@@ -2823,28 +2823,28 @@
     </row>
     <row r="28" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="R28" s="1" t="s">
         <v>23</v>
@@ -2853,16 +2853,16 @@
         <v>1</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="V28" s="2" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="W28" s="2" t="s">
-        <v>275</v>
+        <v>241</v>
       </c>
       <c r="X28" s="2" t="s">
         <v>6</v>
@@ -2873,46 +2873,46 @@
     </row>
     <row r="29" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>4</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="S29" s="2">
         <v>1</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="U29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="V29" s="2" t="s">
-        <v>240</v>
+        <v>214</v>
       </c>
       <c r="W29" s="2" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="X29" s="2" t="s">
         <v>4</v>
@@ -2923,23 +2923,23 @@
     </row>
     <row r="30" spans="1:25" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
       <c r="O30" s="3" t="s">
         <v>1</v>
       </c>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="R30" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S30" s="4">
         <v>3</v>
@@ -2951,10 +2951,10 @@
         <v>14</v>
       </c>
       <c r="V30" s="2" t="s">
-        <v>183</v>
+        <v>272</v>
       </c>
       <c r="W30" s="2" t="s">
-        <v>247</v>
+        <v>220</v>
       </c>
       <c r="X30" s="4" t="s">
         <v>1</v>
@@ -2965,31 +2965,31 @@
     </row>
     <row r="31" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O31" s="1" t="s">
         <v>4</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="S31" s="2">
         <v>1</v>
@@ -3001,10 +3001,10 @@
         <v>14</v>
       </c>
       <c r="V31" s="2" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="W31" s="2" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="X31" s="2" t="s">
         <v>3</v>
@@ -3015,34 +3015,34 @@
     </row>
     <row r="32" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>278</v>
+        <v>244</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="O32" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="S32" s="2">
         <v>1</v>
@@ -3054,10 +3054,10 @@
         <v>14</v>
       </c>
       <c r="V32" s="2" t="s">
-        <v>187</v>
+        <v>273</v>
       </c>
       <c r="W32" s="2" t="s">
-        <v>279</v>
+        <v>245</v>
       </c>
       <c r="X32" s="2" t="s">
         <v>2</v>
@@ -3068,22 +3068,22 @@
     </row>
     <row r="33" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>280</v>
+        <v>246</v>
       </c>
       <c r="O33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="S33" s="2">
         <v>2</v>
@@ -3095,10 +3095,10 @@
         <v>0</v>
       </c>
       <c r="V33" s="2" t="s">
-        <v>188</v>
+        <v>274</v>
       </c>
       <c r="W33" s="2" t="s">
-        <v>281</v>
+        <v>247</v>
       </c>
       <c r="X33" s="2" t="s">
         <v>1</v>
@@ -3109,28 +3109,28 @@
     </row>
     <row r="34" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="S34" s="2">
         <v>2</v>
@@ -3142,10 +3142,10 @@
         <v>0</v>
       </c>
       <c r="V34" s="2" t="s">
-        <v>193</v>
+        <v>290</v>
       </c>
       <c r="W34" s="2" t="s">
-        <v>283</v>
+        <v>249</v>
       </c>
       <c r="X34" s="2" t="s">
         <v>1</v>
@@ -3156,52 +3156,52 @@
     </row>
     <row r="35" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>282</v>
+        <v>248</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>206</v>
+        <v>275</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="S35" s="2">
         <v>1</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="U35" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="V35" s="2" t="s">
-        <v>195</v>
+        <v>276</v>
       </c>
       <c r="W35" s="2" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="X35" s="2" t="s">
         <v>4</v>
@@ -3212,34 +3212,34 @@
     </row>
     <row r="36" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O36" s="1" t="s">
         <v>6</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>205</v>
+        <v>278</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="S36" s="2">
         <v>1</v>
@@ -3248,13 +3248,13 @@
         <v>5</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="W36" s="2" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="X36" s="2" t="s">
         <v>5</v>
@@ -3265,55 +3265,55 @@
     </row>
     <row r="37" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>284</v>
+        <v>250</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O37" s="1" t="s">
         <v>9</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
       <c r="S37" s="2">
         <v>1</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="U37" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="V37" s="2" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="W37" s="2" t="s">
-        <v>285</v>
+        <v>251</v>
       </c>
       <c r="X37" s="2" t="s">
         <v>7</v>
@@ -3324,46 +3324,46 @@
     </row>
     <row r="38" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>220</v>
+        <v>279</v>
       </c>
       <c r="S38" s="2">
         <v>1</v>
@@ -3372,13 +3372,13 @@
         <v>7</v>
       </c>
       <c r="U38" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="W38" s="2" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="X38" s="2" t="s">
         <v>8</v>
@@ -3389,55 +3389,55 @@
     </row>
     <row r="39" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>262</v>
+        <v>233</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>286</v>
+        <v>252</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="S39" s="2">
         <v>1</v>
       </c>
       <c r="T39" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="V39" s="2" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="W39" s="2" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="X39" s="2" t="s">
         <v>6</v>
@@ -3448,52 +3448,52 @@
     </row>
     <row r="40" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>196</v>
+        <v>282</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="S40" s="2">
         <v>1</v>
       </c>
       <c r="T40" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="U40" s="1" t="s">
         <v>1</v>
       </c>
       <c r="V40" s="2" t="s">
-        <v>244</v>
+        <v>283</v>
       </c>
       <c r="W40" s="2" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="X40" s="2" t="s">
         <v>5</v>
@@ -3504,49 +3504,49 @@
     </row>
     <row r="41" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="O41" s="1" t="s">
         <v>9</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="S41" s="2">
         <v>1</v>
       </c>
       <c r="T41" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="U41" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="V41" s="2" t="s">
-        <v>216</v>
+        <v>285</v>
       </c>
       <c r="W41" s="2" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="X41" s="2" t="s">
         <v>6</v>
@@ -3557,25 +3557,25 @@
     </row>
     <row r="42" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I42" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="O42" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="S42" s="2">
         <v>2</v>
@@ -3587,10 +3587,10 @@
         <v>14</v>
       </c>
       <c r="V42" s="2" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="W42" s="2" t="s">
-        <v>247</v>
+        <v>220</v>
       </c>
       <c r="X42" s="2" t="s">
         <v>4</v>

</xml_diff>